<commit_message>
Fixed app in 22a
</commit_message>
<xml_diff>
--- a/tbx/replications/data_61.xlsx
+++ b/tbx/replications/data_61.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0858DD7B-DE2B-4A99-8209-5D57A47F576E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2527D637-0D04-4EB5-B921-13720DAF5D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="946" firstSheet="14" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="946" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="12" r:id="rId1"/>
@@ -19177,15 +19177,15 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B2:O6"/>
+  <dimension ref="B2:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>1582</v>
       </c>
@@ -19198,8 +19198,14 @@
       <c r="E2" s="10" t="s">
         <v>1585</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="37" t="s">
         <v>1331</v>
@@ -19210,8 +19216,15 @@
       <c r="E3" s="37" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I3" s="63" t="s">
+        <v>1602</v>
+      </c>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>1331</v>
       </c>
@@ -19219,34 +19232,21 @@
       <c r="D4" s="50"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>1332</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
-      <c r="M5" t="s">
-        <v>1604</v>
-      </c>
-      <c r="O5" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>1333</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
-      <c r="M6" s="63" t="s">
-        <v>1602</v>
-      </c>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63" t="s">
-        <v>1603</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19329,15 +19329,15 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B2:P6"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="G2" sqref="G2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>1582</v>
       </c>
@@ -19350,8 +19350,14 @@
       <c r="E2" s="10" t="s">
         <v>1585</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="C3" s="37" t="s">
         <v>1331</v>
@@ -19362,8 +19368,11 @@
       <c r="E3" s="37" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>1331</v>
       </c>
@@ -19371,30 +19380,21 @@
       <c r="D4" s="50"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>1332</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
-      <c r="O5" t="s">
-        <v>1606</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>1333</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
-      <c r="O6" t="s">
-        <v>1607</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19408,7 +19408,7 @@
   </sheetPr>
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>